<commit_message>
Reorganized file structure, included named pipe communication files
</commit_message>
<xml_diff>
--- a/MoonkinSpellsCalc.xlsx
+++ b/MoonkinSpellsCalc.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tobi\Documents\Programming\MachineLearning\WowFeralMLSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B872C8FF-96B0-480A-8C50-FF237BC90F4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B38A150-EAB9-4BFB-BFC8-619030C2A53F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="330" windowWidth="25440" windowHeight="15390" xr2:uid="{3C82C9D4-C00F-4035-ADF0-4FCBD7F8A8F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3C82C9D4-C00F-4035-ADF0-4FCBD7F8A8F2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Spell Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Owl Weaving" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="92">
   <si>
     <t>int</t>
   </si>
@@ -168,13 +169,154 @@
   </si>
   <si>
     <t>AP (Agi and wepdps) * 0.96305732 * vers (no moonkin buff, no balance aura)</t>
+  </si>
+  <si>
+    <t>Sunfire only single target</t>
+  </si>
+  <si>
+    <t>Assume: Use spender at lowest energy possible, get refunded 25 energy + 10 energy for gcd, last autoattack was immediately before shapeshift</t>
+  </si>
+  <si>
+    <t>Assume: 0% haste, 0% versatility, 16% mastery</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Time investment</t>
+  </si>
+  <si>
+    <t>At time</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>Moonkin form</t>
+  </si>
+  <si>
+    <t>1.5s</t>
+  </si>
+  <si>
+    <t>0s</t>
+  </si>
+  <si>
+    <t>Caster auto hit</t>
+  </si>
+  <si>
+    <t>(Cat_AP * 3.6) / 6 + Wep_dps</t>
+  </si>
+  <si>
+    <t>1s</t>
+  </si>
+  <si>
+    <t>3.6s attack swing cd, can attack after 4.6 second, basically after switching back to cat form cd is over</t>
+  </si>
+  <si>
+    <t>Cat_AP * 96% * 124.4%</t>
+  </si>
+  <si>
+    <t>Cat form</t>
+  </si>
+  <si>
+    <t>3s</t>
+  </si>
+  <si>
+    <t>179.4% Cat_AP + Wep_dps</t>
+  </si>
+  <si>
+    <t>4.5s</t>
+  </si>
+  <si>
+    <t>Note: 45 energy pooled, at 80 energy after switching back</t>
+  </si>
+  <si>
+    <t>Cat form pooling in same window</t>
+  </si>
+  <si>
+    <t>Pooling</t>
+  </si>
+  <si>
+    <t>Auto hit</t>
+  </si>
+  <si>
+    <t>(Cat_AP * 1.4) / 6</t>
+  </si>
+  <si>
+    <t>2s</t>
+  </si>
+  <si>
+    <t>4s</t>
+  </si>
+  <si>
+    <t>Note: 45 energy pooled, at 80 energy after 4.5s</t>
+  </si>
+  <si>
+    <t>Shred:</t>
+  </si>
+  <si>
+    <t>(7/20) * 1.2 * 0.46 * Cat_AP</t>
+  </si>
+  <si>
+    <t>Note: 7ppm ooc proc, 60apm, 7/60 chance per attack to proc, 3 attacks -&gt; 7/20 multiplier to shred dmg</t>
+  </si>
+  <si>
+    <t>112.653% Cat_AP</t>
+  </si>
+  <si>
+    <t>Assume: Use spender at lowest energy possible, get refunded 25 energy, last autoattack was immediately before shapeshift</t>
+  </si>
+  <si>
+    <t>5s</t>
+  </si>
+  <si>
+    <t>6.5s</t>
+  </si>
+  <si>
+    <t>Note: 65 energy pooled, at 100 energy after switching back</t>
+  </si>
+  <si>
+    <t>Note: 65 energy pooled, at 100 energy after 4.5s</t>
+  </si>
+  <si>
+    <t>6s</t>
+  </si>
+  <si>
+    <t>Sunfire + Starsurge single target (OOC, energy capping)</t>
+  </si>
+  <si>
+    <t>Sunfire + Starsurge single target (MOC)</t>
+  </si>
+  <si>
+    <t>Cat_AP * 96% * 162%</t>
+  </si>
+  <si>
+    <t>358.3% Cat_AP + Wep_dps</t>
+  </si>
+  <si>
+    <t>(7/12) * 1.2 * 0.46 * Cat_AP</t>
+  </si>
+  <si>
+    <t>172.2% * Cat_AP</t>
+  </si>
+  <si>
+    <t>(7/12) * 1.5 * 1.15 * 1.2 * 0.46 * Cat_AP</t>
+  </si>
+  <si>
+    <t>Note: 7ppm ooc proc, 60apm, 10.5/60 chance per attack to proc, 3 attacks -&gt; 7/20 multiplier to shred dmg</t>
+  </si>
+  <si>
+    <t>195.5% * Cat_AP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,8 +331,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,8 +353,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -212,14 +368,114 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -536,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0797F67E-6D93-4A79-A56D-99A60DEC9548}">
   <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,4 +1953,1259 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8131F0-72A4-4EE6-BABE-5A6ECAA66F2D}">
+  <dimension ref="A1:O72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="L12" s="7"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="7"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+      <c r="L17" s="7"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" t="s">
+        <v>72</v>
+      </c>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" t="s">
+        <v>75</v>
+      </c>
+      <c r="L20" s="7"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="10"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="7"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="7"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="7"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="7"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="7"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="15">
+        <v>0</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="7"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="7"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="7"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="7"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="15">
+        <v>0</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="7"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="7"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="7"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="7"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="7"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="15">
+        <v>0</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="7"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="7"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15">
+        <f>1.4+7/12*1.2*0.46</f>
+        <v>1.722</v>
+      </c>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="7"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="7"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="7"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="7"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="7"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="7"/>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="10"/>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="5"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="7"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="7"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="7"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="6"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="7"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="7"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="15">
+        <v>0</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="7"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="7"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="7"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="7"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="15">
+        <v>0</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="7"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="15"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="7"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="7"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="6"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="7"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="7"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" s="15">
+        <v>0</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="7"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="7"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="7"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="7"/>
+      <c r="O67">
+        <f>7/12*1.2*0.46</f>
+        <v>0.32200000000000006</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="7"/>
+      <c r="O68">
+        <f>7/12*1.5*1.15*1.2*0.46+1.4</f>
+        <v>1.9554499999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="7"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+      <c r="J70" s="15"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="7"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="7"/>
+    </row>
+    <row r="72" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>